<commit_message>
Fixed PBI refresh failure by replacing DAX columns in d_time table with PowerQuery custom columns.
</commit_message>
<xml_diff>
--- a/Data/SourceData_Expenses.xlsx
+++ b/Data/SourceData_Expenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EVERYTHING_PROGRAMMING\ProcurementSpendProject\Python_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D5F928-D241-4C27-9170-5C6BA7672028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6924B8A-BC09-4CC3-88D0-C5CE99C352E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5171,8 +5171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0BA6BF-2602-472E-875E-952466AB6E08}">
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6040,7 +6040,9 @@
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
+      <c r="G32" s="3">
+        <v>208.54</v>
+      </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>

</xml_diff>

<commit_message>
Added time selector in Expenses overview as well.
</commit_message>
<xml_diff>
--- a/Data/SourceData_Expenses.xlsx
+++ b/Data/SourceData_Expenses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EVERYTHING_PROGRAMMING\ProcurementSpendProject\Python_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6924B8A-BC09-4CC3-88D0-C5CE99C352E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152A3C52-82CE-4F8A-9EE0-A0BC22C5B761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="202410" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="47">
   <si>
     <t>METROU</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>TERAPIE</t>
-  </si>
-  <si>
-    <t>CARTE</t>
   </si>
   <si>
     <t>MANCAT IN ORAS</t>
@@ -509,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334A57E1-D461-4ED5-9ED5-8FAB77AD8F05}">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,7 +524,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -536,7 +533,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -548,13 +545,13 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>5</v>
@@ -566,13 +563,13 @@
         <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q1" s="1"/>
     </row>
@@ -1239,28 +1236,28 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -1278,31 +1275,31 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="W1" s="1"/>
     </row>
@@ -1614,28 +1611,28 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -1653,28 +1650,28 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="V1" s="1"/>
     </row>
@@ -1971,28 +1968,28 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -2010,25 +2007,25 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U1" s="1"/>
     </row>
@@ -2289,28 +2286,28 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -2328,40 +2325,40 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="Z1" s="1"/>
     </row>
@@ -3335,28 +3332,28 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -3371,25 +3368,25 @@
         <v>2</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>4</v>
@@ -4281,28 +4278,28 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -4317,37 +4314,37 @@
         <v>2</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="X1" s="1"/>
     </row>
@@ -4435,7 +4432,7 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="3">
         <v>71</v>
@@ -5171,7 +5168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0BA6BF-2602-472E-875E-952466AB6E08}">
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -5182,28 +5179,28 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -5218,34 +5215,34 @@
         <v>2</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="W1" s="1"/>
     </row>

</xml_diff>

<commit_message>
Refactoring 7 - Changed data sources in powerbi project, changed embed link in web app, updated the order of etl scripts in batch file
</commit_message>
<xml_diff>
--- a/Data/SourceData_Expenses.xlsx
+++ b/Data/SourceData_Expenses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EVERYTHING_PROGRAMMING\ProcurementSpendProject\Python_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152A3C52-82CE-4F8A-9EE0-A0BC22C5B761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152C2D96-E3AD-403E-8585-D10D32E2D7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="202410" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="202503" sheetId="7" r:id="rId6"/>
     <sheet name="202504" sheetId="8" r:id="rId7"/>
     <sheet name="202505" sheetId="9" r:id="rId8"/>
+    <sheet name="202506" sheetId="11" r:id="rId9"/>
+    <sheet name="202507" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="55">
   <si>
     <t>METROU</t>
   </si>
@@ -173,6 +175,30 @@
   </si>
   <si>
     <t>DAY</t>
+  </si>
+  <si>
+    <t>CASTI TELEFON</t>
+  </si>
+  <si>
+    <t>TUNS</t>
+  </si>
+  <si>
+    <t>GUITAR PEDAL</t>
+  </si>
+  <si>
+    <t>STEAM GAME</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>INSECTICID</t>
+  </si>
+  <si>
+    <t>SPOTIFY</t>
+  </si>
+  <si>
+    <t>LEFT</t>
   </si>
 </sst>
 </file>
@@ -506,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334A57E1-D461-4ED5-9ED5-8FAB77AD8F05}">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -1216,6 +1242,875 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619DC17C-8451-4B36-B5E1-A2697D065D2C}">
+  <dimension ref="A1:X32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3">
+        <v>156.41</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3">
+        <v>49</v>
+      </c>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="U3">
+        <v>21.58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
+        <v>163.76</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1500</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>17.7</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3">
+        <v>3</v>
+      </c>
+      <c r="L7" s="3">
+        <v>23.3</v>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>40</v>
+      </c>
+      <c r="G8" s="3">
+        <v>11.69</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3">
+        <v>49</v>
+      </c>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3">
+        <v>500</v>
+      </c>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>37</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3">
+        <v>25.5</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3">
+        <v>3</v>
+      </c>
+      <c r="L12" s="3">
+        <v>26.5</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3">
+        <v>29</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="H13" s="3">
+        <v>45.5</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3">
+        <v>3</v>
+      </c>
+      <c r="L13" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3">
+        <v>49</v>
+      </c>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3">
+        <v>86.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3">
+        <v>81</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3">
+        <v>14.1</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="V15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3">
+        <v>22.5</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3">
+        <v>74.5</v>
+      </c>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3">
+        <v>11</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3">
+        <v>280</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3">
+        <v>3</v>
+      </c>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3">
+        <v>7.22</v>
+      </c>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3">
+        <v>49</v>
+      </c>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3">
+        <v>86.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="W23">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3">
+        <v>49</v>
+      </c>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3">
+        <v>22</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3">
+        <v>55.76</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3">
+        <v>183.08</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3">
+        <v>3</v>
+      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3">
+        <v>11</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3">
+        <v>10.59</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3">
+        <v>96.33</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3">
+        <v>49</v>
+      </c>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="X31">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3">
+        <v>23.19</v>
+      </c>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5169,7 +6064,7 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6082,4 +6977,865 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8452343C-784B-4521-A961-64C11E0634E8}">
+  <dimension ref="A1:W33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3">
+        <v>79</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
+        <v>142.07</v>
+      </c>
+      <c r="H5" s="3">
+        <v>32</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3">
+        <v>49</v>
+      </c>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
+        <v>23.14</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
+        <v>10.89</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1500</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <v>40</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
+        <v>10.89</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3">
+        <v>10</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3">
+        <v>193.48</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3">
+        <v>600</v>
+      </c>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3">
+        <v>111</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
+        <v>65</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3">
+        <v>56</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3">
+        <v>5</v>
+      </c>
+      <c r="K13" s="3">
+        <v>3</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="T13">
+        <v>48.69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3">
+        <v>298</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3">
+        <v>24.5</v>
+      </c>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3">
+        <v>11</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="U17">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3">
+        <v>87.33</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3">
+        <v>5</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3">
+        <v>32</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3">
+        <v>11.1</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3">
+        <v>3</v>
+      </c>
+      <c r="L21" s="3">
+        <v>34.6</v>
+      </c>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3">
+        <v>24.5</v>
+      </c>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3">
+        <v>10</v>
+      </c>
+      <c r="K22" s="3">
+        <v>3</v>
+      </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3">
+        <v>193</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3">
+        <v>5</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3">
+        <v>49</v>
+      </c>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3">
+        <v>11.59</v>
+      </c>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3">
+        <v>37</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3">
+        <v>205.16</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3">
+        <v>49</v>
+      </c>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3">
+        <v>44</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="V30">
+        <v>764</v>
+      </c>
+      <c r="W30">
+        <v>43.21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>